<commit_message>
Completed Lesson 10 JMeter
</commit_message>
<xml_diff>
--- a/Katalon Projects/Test Scenarios/COOLMATE-001.xlsx
+++ b/Katalon Projects/Test Scenarios/COOLMATE-001.xlsx
@@ -116,7 +116,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +139,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -220,55 +228,40 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -555,7 +548,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,165 +557,165 @@
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:8" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:8" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:8" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+    <row r="5" spans="1:8" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:8" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>